<commit_message>
deleted:    config.json 	deleted:    final.xlsx 	modified:   homeworkchecker v2.5.py 	modified:   "\346\265\213\350\257\225\346\225\260\346\215\256\346\272\220/homework.xlsx"
</commit_message>
<xml_diff>
--- a/测试数据源/homework.xlsx
+++ b/测试数据源/homework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Python\看作业系统\测试数据源\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28ABDFFE-8F35-4287-9638-68AB3AB885F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72478CF-6A0B-429D-BF72-6FEC07B0DE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2952" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3084" yWindow="1548" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>